<commit_message>
evaluation code, CSV and Tableau files
</commit_message>
<xml_diff>
--- a/train_dir/model_param_lookup.xlsx
+++ b/train_dir/model_param_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U\Documents\Minyus\CyclicGen\train_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48497643-4F99-443C-B68B-8EFFEC646CC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719E447-5A4B-4D14-9A63-86BDB4FEA41A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="390" windowWidth="17280" windowHeight="10523" xr2:uid="{AB74A01D-11BE-4729-B775-8040F5A4AA1A}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="17279" windowHeight="10522" xr2:uid="{AB74A01D-11BE-4729-B775-8040F5A4AA1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>2019-04-22T082112</t>
   </si>
@@ -94,6 +94,51 @@
   </si>
   <si>
     <t>max_epochs</t>
+  </si>
+  <si>
+    <t>2019-04-23T083858</t>
+  </si>
+  <si>
+    <t>2019-04-23T141504</t>
+  </si>
+  <si>
+    <t>model_description</t>
+  </si>
+  <si>
+    <t>ours.png</t>
+  </si>
+  <si>
+    <t>base(deep_voxel_flow)</t>
+  </si>
+  <si>
+    <t>[Baseline]  Deep Voxel Flow</t>
+  </si>
+  <si>
+    <t>[Baseline]  CyclicGen</t>
+  </si>
+  <si>
+    <t>[Baseline]  Stage 1 Only</t>
+  </si>
+  <si>
+    <t>[Proposed] CyclicGen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Proposed] CyclicGen: Adapt to Acceleration </t>
+  </si>
+  <si>
+    <t>[Proposed] CyclicGen: Adapt to Acceleration &amp; Extra Cycle Consistency Loss (coef: 0.5)</t>
+  </si>
+  <si>
+    <t>[Proposed] CyclicGen: Extra Cycle Consistency Loss (coef: 0.5)</t>
+  </si>
+  <si>
+    <t>[Proposed] CyclicGen: Adapt to Acceleration &amp; Extra Cycle Consistency Loss (coef: 1.0)</t>
+  </si>
+  <si>
+    <t>[Proposed] CyclicGen: Extra Cycle Consistency Loss (coef: 1.0)</t>
+  </si>
+  <si>
+    <t>[Baseline]  1 Batch Only</t>
   </si>
 </sst>
 </file>
@@ -445,19 +490,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33AB073-814A-490A-8A21-3B38841D75A4}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.46484375" customWidth="1"/>
+    <col min="3" max="3" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="55.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -479,33 +528,24 @@
       <c r="G1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -517,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -525,10 +565,13 @@
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -540,41 +583,47 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -583,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -594,33 +643,39 @@
       <c r="G6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -638,18 +693,21 @@
         <v>5</v>
       </c>
       <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -663,16 +721,19 @@
       <c r="G9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -686,16 +747,19 @@
       <c r="G10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -709,16 +773,19 @@
       <c r="G11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -732,13 +799,16 @@
       <c r="G12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -754,6 +824,87 @@
       </c>
       <c r="G13">
         <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>